<commit_message>
Added Besprechungsprotokoll-2016-11-14 worked on Vorlage-Projektbeschreibung.docx worked on Featurelist & Arbeitspakete.xlsx Added Icon and gimp-files into newly created img & gimp folders
</commit_message>
<xml_diff>
--- a/doc/Arbeitspakete.xlsx
+++ b/doc/Arbeitspakete.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$2:$G$2</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
   <si>
     <t>Arbeitspakete v0.1</t>
   </si>
@@ -40,6 +43,159 @@
   </si>
   <si>
     <t>(in PH)</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Phillip</t>
+  </si>
+  <si>
+    <t>Startseite</t>
+  </si>
+  <si>
+    <t>HTML+CSS</t>
+  </si>
+  <si>
+    <t>Hilfeseite</t>
+  </si>
+  <si>
+    <t>Impressum</t>
+  </si>
+  <si>
+    <t>Spieleseite</t>
+  </si>
+  <si>
+    <t>JS</t>
+  </si>
+  <si>
+    <t>Startseite Spieleauswahl</t>
+  </si>
+  <si>
+    <t>Vorheriges AP</t>
+  </si>
+  <si>
+    <t>Thiago</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Selina</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>JS+PHP+DB</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>Datenbank-Design</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>SQL-Statements definieren und schreiben</t>
+  </si>
+  <si>
+    <t>Teamwahl &amp; Namenswahl &amp; Spielseite laden</t>
+  </si>
+  <si>
+    <t>PHP+DB</t>
+  </si>
+  <si>
+    <t>Spielstatus abrufen &amp; Spielframe laden</t>
+  </si>
+  <si>
+    <t>Tic Tac Toe</t>
+  </si>
+  <si>
+    <t>4-Gewinnt</t>
+  </si>
+  <si>
+    <t>11,12,8</t>
+  </si>
+  <si>
+    <t>Vorschaubilder &amp; Titelbild zeichnen</t>
+  </si>
+  <si>
+    <t>Chat</t>
+  </si>
+  <si>
+    <t>Teamchat</t>
+  </si>
+  <si>
+    <t>Global-Chat</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>Domain kaufen und Server einrichten</t>
+  </si>
+  <si>
+    <t>Spieltimer implementieren</t>
+  </si>
+  <si>
+    <t>11,12,8,0,</t>
+  </si>
+  <si>
+    <t>Reset des Spiels</t>
+  </si>
+  <si>
+    <t>Gewinnüberprüfung 4 Gewinnt</t>
+  </si>
+  <si>
+    <t>15,8,12</t>
+  </si>
+  <si>
+    <t>Gewinnüberprüfung Tic-Tac-Toe</t>
+  </si>
+  <si>
+    <t>15,8,11</t>
+  </si>
+  <si>
+    <t>Ergebnisanzeige</t>
+  </si>
+  <si>
+    <t>PHP+JS+DB</t>
+  </si>
+  <si>
+    <t>Anzeige Zwischenergebnis</t>
+  </si>
+  <si>
+    <t>Spieler aus der DB entfernen -&gt; wenn er Spieleseite verlässt</t>
+  </si>
+  <si>
+    <t>Testen</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>PM (noch auf anderes aufteilen)</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Alle</t>
+  </si>
+  <si>
+    <t>1,8,9</t>
+  </si>
+  <si>
+    <t>Ausführung Spielzug des Spielers</t>
+  </si>
+  <si>
+    <t>Spielzug des Teams ausführen + Anzeige</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -63,7 +219,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -73,6 +229,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -89,10 +251,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -407,21 +570,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" customWidth="1"/>
     <col min="3" max="3" width="109" customWidth="1"/>
     <col min="4" max="4" width="8.21875" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -429,144 +595,630 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17">
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19">
+        <v>15.8</v>
+      </c>
+      <c r="G19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22">
+        <v>17.18</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26">
+        <v>8</v>
+      </c>
+      <c r="G26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>24</v>
       </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27">
+        <v>30</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28">
+        <v>50</v>
+      </c>
+      <c r="E28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:G2">
+    <sortState ref="A3:G28">
+      <sortCondition ref="A2"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Logo-Short xcf & png Changed BG Color Of Logo to transparent Added Basic Information to Readme.md
</commit_message>
<xml_diff>
--- a/doc/Arbeitspakete.xlsx
+++ b/doc/Arbeitspakete.xlsx
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15:H16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
rendered Images for actual game and renamed and moved some files
</commit_message>
<xml_diff>
--- a/doc/Arbeitspakete.xlsx
+++ b/doc/Arbeitspakete.xlsx
@@ -572,15 +572,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.109375" customWidth="1"/>
     <col min="2" max="2" width="11.21875" customWidth="1"/>
-    <col min="3" max="3" width="109" customWidth="1"/>
+    <col min="3" max="3" width="48.5546875" customWidth="1"/>
     <col min="4" max="4" width="8.21875" customWidth="1"/>
     <col min="5" max="5" width="12.109375" customWidth="1"/>
     <col min="6" max="6" width="13.21875" customWidth="1"/>

</xml_diff>

<commit_message>
Fixed index page reloading on resize bug Added aktueller-stand_2017-01.23 Changed Arbeitspakete to version 2.0 Updated Abschlussdokument
</commit_message>
<xml_diff>
--- a/doc/Arbeitspakete.xlsx
+++ b/doc/Arbeitspakete.xlsx
@@ -1,16 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="v1.0" sheetId="1" r:id="rId1"/>
+    <sheet name="v2.0" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$2:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">v1.0!$A$2:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">v2.0!$A$2:$H$2</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -22,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
-  <si>
-    <t>Arbeitspakete v0.1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="142">
   <si>
     <t>ID</t>
   </si>
@@ -196,6 +195,261 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>System-ID</t>
+  </si>
+  <si>
+    <t>Thiago Gumhold</t>
+  </si>
+  <si>
+    <t>Phillip Schermann</t>
+  </si>
+  <si>
+    <t>Phillip Schermann &amp; Thiago Gumhold</t>
+  </si>
+  <si>
+    <t>Alexander Dietrich &amp; Phillip Schermann</t>
+  </si>
+  <si>
+    <t>Phillip Schermann &amp; Selina Brinnich</t>
+  </si>
+  <si>
+    <t>Selina Brinnich &amp; Thiago Gumhold</t>
+  </si>
+  <si>
+    <t>SQL Statements definieren und schreiben</t>
+  </si>
+  <si>
+    <t>Selina Brinnich</t>
+  </si>
+  <si>
+    <t>11 &amp; 55</t>
+  </si>
+  <si>
+    <t>Phillip Schermann &amp; Selina Brinnich &amp; Thiago Gumhold</t>
+  </si>
+  <si>
+    <t>Alexander Dietrich</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>Recherche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  In PHP-Timer einlesen</t>
+  </si>
+  <si>
+    <t>9.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Timings festlegen</t>
+  </si>
+  <si>
+    <t>9.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Timer programmieren</t>
+  </si>
+  <si>
+    <t>106 &amp; 110</t>
+  </si>
+  <si>
+    <t>1 &amp; 11 &amp; 12 &amp; 55</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Websockets/Ajax einlesen</t>
+  </si>
+  <si>
+    <t>Alexander Dietrich &amp; Phillip Schermann &amp; Selina Brinnich &amp; Thiago Gumhold</t>
+  </si>
+  <si>
+    <t>10.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  PHP einlesen</t>
+  </si>
+  <si>
+    <t>10.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Datenbankzugriff programmieren</t>
+  </si>
+  <si>
+    <t>10.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Team- und Namenswahl implementieren</t>
+  </si>
+  <si>
+    <t>10.5</t>
+  </si>
+  <si>
+    <t>JS+PHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Spielseite laden</t>
+  </si>
+  <si>
+    <t>11 &amp; 19 &amp; 124</t>
+  </si>
+  <si>
+    <t>11 &amp; 15 &amp; 16 &amp; 55</t>
+  </si>
+  <si>
+    <t>12.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Spielstatus Tic-Tac-Toe</t>
+  </si>
+  <si>
+    <t>12.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Spielstatus 4-Gewinnt</t>
+  </si>
+  <si>
+    <t>Tic-Tac-Toe</t>
+  </si>
+  <si>
+    <t>PHP+BD</t>
+  </si>
+  <si>
+    <t>GewinnÃ¼berprÃ¼fung Tic-Tac-Toe</t>
+  </si>
+  <si>
+    <t>11 &amp; 15 &amp; 19 &amp; 160</t>
+  </si>
+  <si>
+    <t>AusfÃ¼hrung Spielzug Spielers</t>
+  </si>
+  <si>
+    <t>11 &amp; 15 &amp; 16</t>
+  </si>
+  <si>
+    <t>Spielzug des Teams ausfÃ¼hren + Anzeige</t>
+  </si>
+  <si>
+    <t>GewinnÃ¼berprÃ¼fung 4-Gewinnt</t>
+  </si>
+  <si>
+    <t>Alexander Dietrich &amp; Selina Brinnich</t>
+  </si>
+  <si>
+    <t>21 &amp; 22 &amp; 162</t>
+  </si>
+  <si>
+    <t>Spieler aus der DB entfernen wenn er die Spielseite verlÃ¤sst</t>
+  </si>
+  <si>
+    <t>21.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  PHP Sessions einlesen</t>
+  </si>
+  <si>
+    <t>21.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Spieler aus DB entfernen wenn er die Seite verlÃ¤sst implementieren</t>
+  </si>
+  <si>
+    <t>Global Chat</t>
+  </si>
+  <si>
+    <t>24.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  TestfÃ¤lle schreiben</t>
+  </si>
+  <si>
+    <t>24.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Progressionstesten</t>
+  </si>
+  <si>
+    <t>24.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Regressionstesten</t>
+  </si>
+  <si>
+    <t>Projektmanagement</t>
+  </si>
+  <si>
+    <t>25.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Projektstart</t>
+  </si>
+  <si>
+    <t>25.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Projektplanung</t>
+  </si>
+  <si>
+    <t>25.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Projektdokumentation</t>
+  </si>
+  <si>
+    <t>25.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Projektkoordination</t>
+  </si>
+  <si>
+    <t>25.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Projektcontrolling</t>
+  </si>
+  <si>
+    <t>25.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Projektabschluss</t>
+  </si>
+  <si>
+    <t>Vorherige APs</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>12 &amp; 15 &amp; 16 &amp; 55</t>
+  </si>
+  <si>
+    <t>13 &amp; 15 &amp; 16 &amp; 55</t>
+  </si>
+  <si>
+    <t>11 &amp; 16  &amp; 19 &amp; 124</t>
+  </si>
+  <si>
+    <t>Tats. Aufwand</t>
+  </si>
+  <si>
+    <t>Aufwand (in Personenstunden)</t>
+  </si>
+  <si>
+    <t>Arbeitspakete v2.0</t>
+  </si>
+  <si>
+    <t>Arbeitspakete v1.0</t>
+  </si>
+  <si>
+    <t>Differenz</t>
+  </si>
+  <si>
+    <t>41 &amp; 42</t>
   </si>
 </sst>
 </file>
@@ -251,11 +505,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -570,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,360 +844,361 @@
     <col min="1" max="1" width="4.109375" customWidth="1"/>
     <col min="2" max="2" width="11.21875" customWidth="1"/>
     <col min="3" max="3" width="48.5546875" customWidth="1"/>
-    <col min="4" max="4" width="8.21875" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="12.109375" customWidth="1"/>
     <col min="6" max="6" width="13.21875" customWidth="1"/>
     <col min="7" max="7" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="I2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
         <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9">
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10">
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
       <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
       <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
       </c>
       <c r="D12">
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12">
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
         <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
       </c>
       <c r="D13">
         <v>15</v>
       </c>
       <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" t="s">
         <v>18</v>
       </c>
-      <c r="F13" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14">
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14">
         <v>4</v>
       </c>
       <c r="G14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15">
         <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15">
         <v>4</v>
       </c>
       <c r="G15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>13</v>
       </c>
       <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
         <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
       </c>
       <c r="D16">
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F16">
         <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -942,22 +1206,22 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17">
         <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F17">
         <v>4</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -965,22 +1229,22 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18">
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -988,22 +1252,22 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19">
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F19">
         <v>15.8</v>
       </c>
       <c r="G19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1011,22 +1275,22 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20">
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1034,22 +1298,22 @@
         <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21">
         <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1057,22 +1321,22 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22">
         <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F22">
         <v>17.18</v>
       </c>
       <c r="G22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1080,22 +1344,22 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D23">
         <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1103,22 +1367,22 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" t="s">
         <v>46</v>
-      </c>
-      <c r="C24" t="s">
-        <v>47</v>
       </c>
       <c r="D24">
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1126,22 +1390,22 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25">
         <v>10</v>
       </c>
       <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" t="s">
         <v>18</v>
-      </c>
-      <c r="F25" t="s">
-        <v>31</v>
-      </c>
-      <c r="G25" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1149,22 +1413,22 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26">
         <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F26">
         <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1172,22 +1436,22 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27">
         <v>30</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1195,22 +1459,22 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
         <v>50</v>
-      </c>
-      <c r="C28" t="s">
-        <v>51</v>
       </c>
       <c r="D28">
         <v>50</v>
       </c>
       <c r="E28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F28">
         <v>0</v>
       </c>
       <c r="G28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1222,4 +1486,1360 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="7.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" customWidth="1"/>
+    <col min="8" max="8" width="68.88671875" customWidth="1"/>
+    <col min="11" max="11" width="44.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
+        <v>55</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>1</v>
+      </c>
+      <c r="B5" s="6">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>2</v>
+      </c>
+      <c r="B6" s="6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>3</v>
+      </c>
+      <c r="B7" s="6">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H7" t="s">
+        <v>59</v>
+      </c>
+      <c r="K7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.11805555555555557</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>11</v>
+      </c>
+      <c r="B9" s="6">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="8">
+        <v>55</v>
+      </c>
+      <c r="H9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>12</v>
+      </c>
+      <c r="B10" s="6">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>5</v>
+      </c>
+      <c r="B11" s="6">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.125</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>68</v>
+      </c>
+      <c r="K11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>19</v>
+      </c>
+      <c r="B12" s="6">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="8">
+        <v>55</v>
+      </c>
+      <c r="H12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>106</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H13" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>110</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14" s="8">
+        <v>55</v>
+      </c>
+      <c r="H14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>113</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
+        <v>9</v>
+      </c>
+      <c r="B16" s="6">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H16" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>121</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H17" t="s">
+        <v>80</v>
+      </c>
+      <c r="K17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>124</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H18" t="s">
+        <v>80</v>
+      </c>
+      <c r="K18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
+        <v>126</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="9">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8">
+        <v>124</v>
+      </c>
+      <c r="H19" t="s">
+        <v>63</v>
+      </c>
+      <c r="K19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
+        <v>128</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="G20" s="8">
+        <v>124</v>
+      </c>
+      <c r="H20" t="s">
+        <v>58</v>
+      </c>
+      <c r="K20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>130</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="G21" s="8">
+        <v>124</v>
+      </c>
+      <c r="H21" t="s">
+        <v>58</v>
+      </c>
+      <c r="K21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
+        <v>20</v>
+      </c>
+      <c r="B22" s="6">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H22" t="s">
+        <v>63</v>
+      </c>
+      <c r="K22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <v>13</v>
+      </c>
+      <c r="B23" s="6">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" t="s">
+        <v>68</v>
+      </c>
+      <c r="K23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
+        <v>160</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="H24" t="s">
+        <v>65</v>
+      </c>
+      <c r="K24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
+        <v>162</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="H25" t="s">
+        <v>65</v>
+      </c>
+      <c r="K25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
+        <v>15</v>
+      </c>
+      <c r="B26" s="6">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E26">
+        <v>6</v>
+      </c>
+      <c r="F26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="8">
+        <v>4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>59</v>
+      </c>
+      <c r="K26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
+        <v>22</v>
+      </c>
+      <c r="B27" s="6">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0.125</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H27" t="s">
+        <v>68</v>
+      </c>
+      <c r="K27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
+        <v>25</v>
+      </c>
+      <c r="B28" s="6">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0.15277777777777776</v>
+      </c>
+      <c r="E28">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H28" t="s">
+        <v>63</v>
+      </c>
+      <c r="K28" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
+        <v>26</v>
+      </c>
+      <c r="B29" s="6">
+        <v>16</v>
+      </c>
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0.15277777777777776</v>
+      </c>
+      <c r="E29">
+        <v>10</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H29" t="s">
+        <v>65</v>
+      </c>
+      <c r="K29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="8">
+        <v>27</v>
+      </c>
+      <c r="B30" s="6">
+        <v>17</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H30" t="s">
+        <v>61</v>
+      </c>
+      <c r="K30" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="8">
+        <v>16</v>
+      </c>
+      <c r="B31" s="6">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="E31">
+        <v>15</v>
+      </c>
+      <c r="F31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" s="8">
+        <v>4</v>
+      </c>
+      <c r="H31" t="s">
+        <v>59</v>
+      </c>
+      <c r="K31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="8">
+        <v>21</v>
+      </c>
+      <c r="B32" s="6">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0.125</v>
+      </c>
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="H32" t="s">
+        <v>104</v>
+      </c>
+      <c r="K32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
+        <v>24</v>
+      </c>
+      <c r="B33" s="6">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H33" t="s">
+        <v>62</v>
+      </c>
+      <c r="K33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
+        <v>28</v>
+      </c>
+      <c r="B34" s="6">
+        <v>21</v>
+      </c>
+      <c r="C34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34">
+        <v>6</v>
+      </c>
+      <c r="F34" t="s">
+        <v>59</v>
+      </c>
+      <c r="G34" s="8">
+        <v>9</v>
+      </c>
+      <c r="H34" t="s">
+        <v>60</v>
+      </c>
+      <c r="K34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="8">
+        <v>140</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H35" t="s">
+        <v>80</v>
+      </c>
+      <c r="K35" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
+        <v>143</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="G36" s="8">
+        <v>140</v>
+      </c>
+      <c r="H36" t="s">
+        <v>60</v>
+      </c>
+      <c r="K36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="8">
+        <v>18</v>
+      </c>
+      <c r="B37" s="6">
+        <v>22</v>
+      </c>
+      <c r="C37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="9">
+        <v>0.3125</v>
+      </c>
+      <c r="E37">
+        <v>30</v>
+      </c>
+      <c r="F37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G37" s="8">
+        <v>4</v>
+      </c>
+      <c r="H37" t="s">
+        <v>68</v>
+      </c>
+      <c r="K37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="8">
+        <v>17</v>
+      </c>
+      <c r="B38" s="6">
+        <v>23</v>
+      </c>
+      <c r="C38" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38">
+        <v>10</v>
+      </c>
+      <c r="F38" t="s">
+        <v>68</v>
+      </c>
+      <c r="G38" s="8">
+        <v>18</v>
+      </c>
+      <c r="H38" t="s">
+        <v>68</v>
+      </c>
+      <c r="K38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="8">
+        <v>29</v>
+      </c>
+      <c r="B39" s="6">
+        <v>24</v>
+      </c>
+      <c r="C39" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39">
+        <v>30</v>
+      </c>
+      <c r="F39" t="s">
+        <v>59</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H39" t="s">
+        <v>80</v>
+      </c>
+      <c r="K39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="8">
+        <v>36</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="9">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="E40">
+        <v>6</v>
+      </c>
+      <c r="F40" t="s">
+        <v>59</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H40" t="s">
+        <v>60</v>
+      </c>
+      <c r="K40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="8">
+        <v>37</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="9">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="E41">
+        <v>14</v>
+      </c>
+      <c r="F41" t="s">
+        <v>59</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H41" t="s">
+        <v>80</v>
+      </c>
+      <c r="K41" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="8">
+        <v>38</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="9">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E42">
+        <v>10</v>
+      </c>
+      <c r="F42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H42" t="s">
+        <v>80</v>
+      </c>
+      <c r="K42" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="8">
+        <v>35</v>
+      </c>
+      <c r="B43" s="6">
+        <v>25</v>
+      </c>
+      <c r="C43" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43">
+        <v>50</v>
+      </c>
+      <c r="F43" t="s">
+        <v>58</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H43" t="s">
+        <v>58</v>
+      </c>
+      <c r="K43" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="8">
+        <v>40</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" t="s">
+        <v>49</v>
+      </c>
+      <c r="D44" s="9">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="E44">
+        <v>10</v>
+      </c>
+      <c r="F44" t="s">
+        <v>58</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H44" t="s">
+        <v>58</v>
+      </c>
+      <c r="K44" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="8">
+        <v>82</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="9">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="E45">
+        <v>10</v>
+      </c>
+      <c r="F45" t="s">
+        <v>58</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H45" t="s">
+        <v>58</v>
+      </c>
+      <c r="K45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="8">
+        <v>43</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="9">
+        <v>0.17361111111111113</v>
+      </c>
+      <c r="E46">
+        <v>10</v>
+      </c>
+      <c r="F46" t="s">
+        <v>58</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H46" t="s">
+        <v>58</v>
+      </c>
+      <c r="K46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="8">
+        <v>42</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="9">
+        <v>0.15972222222222224</v>
+      </c>
+      <c r="E47">
+        <v>5</v>
+      </c>
+      <c r="F47" t="s">
+        <v>58</v>
+      </c>
+      <c r="G47" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H47" t="s">
+        <v>58</v>
+      </c>
+      <c r="K47" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="8">
+        <v>41</v>
+      </c>
+      <c r="B48" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" s="9">
+        <v>0.20486111111111113</v>
+      </c>
+      <c r="E48">
+        <v>10</v>
+      </c>
+      <c r="F48" t="s">
+        <v>58</v>
+      </c>
+      <c r="G48" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="H48" t="s">
+        <v>58</v>
+      </c>
+      <c r="K48" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="8">
+        <v>44</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="F49" t="s">
+        <v>58</v>
+      </c>
+      <c r="G49" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H49" t="s">
+        <v>58</v>
+      </c>
+      <c r="K49" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D50" s="10"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:I2"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>